<commit_message>
updated writetoexcel function for webdata to write in multiple tabs
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Canine_Filter_Breed-AmerStaffd.xlsx
+++ b/InputFiles/TC02_Canine_Filter_Breed-AmerStaffd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135A7C2E-58D1-48C8-88AF-D89907041408}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E3FD0E-DBF8-4E27-B2DE-DA09B294B7FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>WebExcel</t>
   </si>
@@ -42,9 +42,6 @@
     <t>dbExcel</t>
   </si>
   <si>
-    <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN ['American Staffordshire Terrier'] WITH DISTINCT c AS c, p, s, demo, diag RETURN coalesce(c.case_id,'') AS `Case ID` , coalesce(s.clinical_study_designation,'') AS `Study Code` , coalesce(s.clinical_study_type,'') AS  `Study Type`, coalesce(demo.breed,'') AS Breed , coalesce(diag.disease_term,'') AS Diagnosis , coalesce(diag.stage_of_disease,'') AS `Stage of Disease` ,  coalesce(demo.patient_age_at_enrollment,'') AS Age , coalesce(demo.sex,'') AS Sex , coalesce(demo.neutered_indicator,'') AS  `Neutered Status`</t>
-  </si>
-  <si>
     <t>TC02_Canine_Filter_Breed-AmerStaffd_Neo4jData.xlsx</t>
   </si>
   <si>
@@ -55,6 +52,41 @@
   </si>
   <si>
     <t>MATCH (s:study) WITH COLLECT(DISTINCT(s.clinical_study_designation)) AS all_studies MATCH (d:demographic) WITH COLLECT(DISTINCT(d.breed)) AS all_breeds, COLLECT(DISTINCT(d.sex)) AS all_sexes, all_studies MATCH (d:diagnosis) WITH COLLECT(DISTINCT(d.disease_term)) AS all_diseases, all_breeds, all_sexes, all_studies MATCH (p:program)&lt;-[*]-(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis) WHERE demo.breed IN['American Staffordshire Terrier']  OPTIONAL MATCH (f:file)-[*]-&gt;(c), (samp:sample)-[*]-&gt;(c) WITH DISTINCT c AS c, p, s, demo, diag, f, samp RETURN count(DISTINCT(f)) as number_of_files , count(DISTINCT(samp)) as number_of_sample , count(DISTINCT(c.case_id)) as number_of_cases , count(DISTINCT(s.clinical_study_designation)) as number_of_study</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) WHERE demo.breed IN ['American Staffordshire Terrier'] WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(c.case_id, '') AS `Case ID`, 
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['American Staffordshire Terrier']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co
+RETURN  coalesce(c.case_id, '') AS `Case ID` ,
+        coalesce(s.clinical_study_designation, '') AS `Study Code` ,
+        coalesce(s.clinical_study_type, '') AS  `Study Type`,
+        coalesce(demo.breed, '') AS Breed ,
+        coalesce(diag.disease_term, '') AS Diagnosis ,
+        coalesce(diag.stage_of_disease, '') AS `Stage of Disease` ,
+        coalesce(demo.patient_age_at_enrollment, '') AS Age ,
+        coalesce(demo.sex, '') AS Sex ,
+        coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
+        coalesce(demo.weight, '') AS `Weight (kg)`,
+        coalesce(diag.best_response, '') AS `Response to Treatment`,
+        coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
 </sst>
 </file>
@@ -424,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,7 +467,7 @@
     <col min="1" max="1" width="75.81640625" customWidth="1"/>
     <col min="2" max="2" width="255.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="70.26953125" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" customWidth="1"/>
+    <col min="4" max="4" width="46.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -443,7 +475,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -452,18 +484,32 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="261" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated tab queries in separate variables; neo4j export works fine
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Canine_Filter_Breed-AmerStaffd.xlsx
+++ b/InputFiles/TC02_Canine_Filter_Breed-AmerStaffd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E3FD0E-DBF8-4E27-B2DE-DA09B294B7FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E87207E-4EA1-4644-A139-767C5CA8C2EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>WebExcel</t>
   </si>
@@ -87,6 +87,37 @@
         coalesce(demo.weight, '') AS `Weight (kg)`,
         coalesce(diag.best_response, '') AS `Response to Treatment`,
         coalesce(co.cohort_description, '') AS `Cohort`</t>
+  </si>
+  <si>
+    <t>TabName</t>
+  </si>
+  <si>
+    <t>CasesTab</t>
+  </si>
+  <si>
+    <t>SamplesTab</t>
+  </si>
+  <si>
+    <t>FilesTab</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE demo.breed IN ['American Staffordshire Terrier']
+OPTIONAL MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+WITH DISTINCT f, parent, c, demo, diag, s
+RETURN  coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_size, '') AS `Size`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed , 
+        coalesce(diag.disease_term,'') AS Diagnosis , 
+        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
   </si>
 </sst>
 </file>
@@ -456,59 +487,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="75.81640625" customWidth="1"/>
-    <col min="2" max="2" width="255.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.26953125" customWidth="1"/>
-    <col min="4" max="4" width="46.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.81640625" customWidth="1"/>
+    <col min="3" max="3" width="123.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="70.26953125" customWidth="1"/>
+    <col min="5" max="5" width="46.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="261" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="217.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed variables and query errors in Bread from TC01 to TC30
</commit_message>
<xml_diff>
--- a/InputFiles/TC02_Canine_Filter_Breed-AmerStaffd.xlsx
+++ b/InputFiles/TC02_Canine_Filter_Breed-AmerStaffd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1777202-42DE-4192-9A48-01F72694EA5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B203BA-E35A-4CEA-BB21-9C69DBD479B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="28680" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -69,6 +69,18 @@
         coalesce(samp.sample_preservation, '') AS `Sample Preservation`</t>
   </si>
   <si>
+    <t>TabName</t>
+  </si>
+  <si>
+    <t>CasesTab</t>
+  </si>
+  <si>
+    <t>SamplesTab</t>
+  </si>
+  <si>
+    <t>FilesTab</t>
+  </si>
+  <si>
     <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
 WHERE demo.breed IN ['American Staffordshire Terrier']
 MATCH (c)&lt;--(diag:diagnosis)
@@ -85,20 +97,7 @@
         coalesce(demo.sex, '') AS Sex ,
         coalesce(demo.neutered_indicator, '') AS `Neutered Status`,
         coalesce(demo.weight, '') AS `Weight (kg)`,
-        coalesce(diag.best_response, '') AS `Response to Treatment`,
-        coalesce(co.cohort_description, '') AS `Cohort`</t>
-  </si>
-  <si>
-    <t>TabName</t>
-  </si>
-  <si>
-    <t>CasesTab</t>
-  </si>
-  <si>
-    <t>SamplesTab</t>
-  </si>
-  <si>
-    <t>FilesTab</t>
+        coalesce(diag.best_response, '') AS `Response to Treatment</t>
   </si>
   <si>
     <t>MATCH (f:file)--&gt;(parent)
@@ -116,8 +115,8 @@
         coalesce(f.file_size, '') AS `Size`,
         coalesce(c.case_id, '') AS `Case ID`, 
         coalesce(demo.breed,'') AS Breed , 
-        coalesce(diag.disease_term,'') AS Diagnosis , 
-        coalesce(s.clinical_study_designation,'') AS `Study Code`</t>
+        coalesce(diag.disease_term,'') AS Diagnosis,
+        coalesce(co.cohort_description, '') AS `Cohort`</t>
   </si>
 </sst>
 </file>
@@ -489,22 +488,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.81640625" customWidth="1"/>
-    <col min="3" max="3" width="123.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="70.26953125" customWidth="1"/>
-    <col min="5" max="5" width="46.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.77734375" customWidth="1"/>
+    <col min="3" max="3" width="123.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="70.21875" customWidth="1"/>
+    <col min="5" max="5" width="46.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -519,12 +518,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
@@ -536,9 +535,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="216" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -553,9 +552,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>

</xml_diff>